<commit_message>
Modifying simple cascade workbook
Code labels and full names added for transitions in simple cascade
workbook.
</commit_message>
<xml_diff>
--- a/optima/cascade-simple.xlsx
+++ b/optima/cascade-simple.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
-    <sheet name="Transition Rates" sheetId="3" r:id="rId3"/>
+    <sheet name="Transition Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>Code Label</t>
   </si>
@@ -112,6 +112,93 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>Sheet Label</t>
+  </si>
+  <si>
+    <t>Vaccination Rate</t>
+  </si>
+  <si>
+    <t>Infection Rate (Vaccinated)</t>
+  </si>
+  <si>
+    <t>LTBI Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>LTBI-TB Progression Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>LTBI Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>LTBI-TB Progression Rate (Treated)</t>
+  </si>
+  <si>
+    <t>LTBI Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>TB Treatment Uptake Rate</t>
+  </si>
+  <si>
+    <t>TB Death Rate (Untreated)</t>
+  </si>
+  <si>
+    <t>TB Treatment Abandonment Rate</t>
+  </si>
+  <si>
+    <t>TB Treatment Success Rate</t>
+  </si>
+  <si>
+    <t>TB Death Rate (Treated)</t>
+  </si>
+  <si>
+    <t>Reinfection Rate (Recovered)</t>
+  </si>
+  <si>
+    <t>Infection Rate (Susceptible)</t>
+  </si>
+  <si>
+    <t>v_rate</t>
+  </si>
+  <si>
+    <t>infs_rate</t>
+  </si>
+  <si>
+    <t>infv_rate</t>
+  </si>
+  <si>
+    <t>ltyes_rate</t>
+  </si>
+  <si>
+    <t>ltno_rate</t>
+  </si>
+  <si>
+    <t>ltsuc_rate</t>
+  </si>
+  <si>
+    <t>ltup_rate</t>
+  </si>
+  <si>
+    <t>lttp_rate</t>
+  </si>
+  <si>
+    <t>acyes_rate</t>
+  </si>
+  <si>
+    <t>acno_rate</t>
+  </si>
+  <si>
+    <t>acud_rate</t>
+  </si>
+  <si>
+    <t>acsuc_rate</t>
+  </si>
+  <si>
+    <t>actd_rate</t>
+  </si>
+  <si>
+    <t>infr_rate</t>
   </si>
 </sst>
 </file>
@@ -174,8 +261,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,85 +572,85 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -574,39 +663,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="5.77734375" customWidth="1"/>
+    <col min="1" max="9" width="5.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -614,83 +703,53 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
         <v>27</v>
       </c>
@@ -699,14 +758,9 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
         <v>29</v>
       </c>
@@ -718,29 +772,14 @@
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -750,12 +789,186 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial loading of parameter names
Project settings now stores link_specs dictionary that maps tag to
parameter name and full name of corresponding transition.
However, it may be more useful in the model to propagate from parameter
name to tag to actual compartment link...
</commit_message>
<xml_diff>
--- a/optima/cascade-simple.xlsx
+++ b/optima/cascade-simple.xlsx
@@ -114,9 +114,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>Sheet Label</t>
-  </si>
-  <si>
     <t>Vaccination Rate</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>infr_rate</t>
+  </si>
+  <si>
+    <t>Tag</t>
   </si>
 </sst>
 </file>
@@ -792,19 +792,19 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -818,10 +818,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -829,10 +829,10 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -840,10 +840,10 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -851,10 +851,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -862,10 +862,10 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -873,10 +873,10 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -884,10 +884,10 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -895,10 +895,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -906,10 +906,10 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -917,10 +917,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -928,10 +928,10 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -939,10 +939,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -950,10 +950,10 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -961,10 +961,10 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New characteristics sheet in cascade workbook
Cascade workbooks now have a "Cascade Characteristics" worksheet, which
aims to define arbitrary characteristics in terms of compartment
population sums, normalised by a pre-defined denominator where
necessary.
This should help in defining prevalence and other more complicated
metrics. See cascade workbooks in this commit for examples.
</commit_message>
<xml_diff>
--- a/optima/cascade-simple.xlsx
+++ b/optima/cascade-simple.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
-    <sheet name="Transitions" sheetId="2" r:id="rId2"/>
-    <sheet name="Transition Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Cascade Characteristics" sheetId="4" r:id="rId2"/>
+    <sheet name="Transitions" sheetId="2" r:id="rId3"/>
+    <sheet name="Transition Parameters" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Code Label</t>
   </si>
@@ -199,6 +200,24 @@
   </si>
   <si>
     <t>Tag</t>
+  </si>
+  <si>
+    <t>Includes</t>
+  </si>
+  <si>
+    <t>lt_inf</t>
+  </si>
+  <si>
+    <t>ac_inf</t>
+  </si>
+  <si>
+    <t>Latent Infections</t>
+  </si>
+  <si>
+    <t>Active Infections</t>
+  </si>
+  <si>
+    <t>Denominator</t>
   </si>
 </sst>
 </file>
@@ -572,7 +591,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,6 +679,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -787,11 +869,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Starting custom migration infrastructure
So far, this just involves extra matrices on the 'population
transitions' worksheet in the project databook.
However, it seems that this too will need transition formatting to be
decided. So it might need to be postponed...
</commit_message>
<xml_diff>
--- a/optima/cascade-simple.xlsx
+++ b/optima/cascade-simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -682,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,7 +874,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Major changes to cascade terminology
Rather than naming cascade-workbook sheets 'Cascade Characteristics' and
'Transition Parameters', we simplify them into 'Characteristics' and
'Parameters', roughly translating into 'Outputs' and 'Inputs'.
(Very roughly! Be mindful of subtleties.)
So the core four sheets of a cascade workbook are currently
'Compartments', 'Transitions', 'Characteristics' and 'Parameters', with
the former two defining the cascade network and the latter two
establishing variables relevant to the Model.
In practice, this is setting up the Parameters sheet to include
'untagged' variables (i.e. ones that do not directly represent
transition rates). See the current cascade.xlsx for stubbed
infectiousness examples.
Note: A few more ModelPopulation methods have been commented out as they
are unused diagnostics or superseded by processes at the Model level.
</commit_message>
<xml_diff>
--- a/optima/cascade-simple.xlsx
+++ b/optima/cascade-simple.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
-    <sheet name="Cascade Characteristics" sheetId="4" r:id="rId2"/>
-    <sheet name="Transitions" sheetId="2" r:id="rId3"/>
-    <sheet name="Transition Parameters" sheetId="3" r:id="rId4"/>
+    <sheet name="Transitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Characteristics" sheetId="4" r:id="rId3"/>
+    <sheet name="Parameters" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -199,9 +199,6 @@
     <t>infr_rate</t>
   </si>
   <si>
-    <t>Tag</t>
-  </si>
-  <si>
     <t>Includes</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>Denominator</t>
+  </si>
+  <si>
+    <t>Transition Tag</t>
   </si>
 </sst>
 </file>
@@ -680,6 +680,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="5.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -702,18 +830,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -724,10 +852,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -738,134 +866,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="5.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -873,20 +873,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>